<commit_message>
tratativa de erro End of file quando nao é inserido input
</commit_message>
<xml_diff>
--- a/lugares_visitar.xlsx
+++ b/lugares_visitar.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25217"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8ef347e2f94c6c43/Documentos/Locais para Sair/lugares-para-sair/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="81" documentId="8_{DCB34105-0091-4572-A59E-812606D8BD9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C530F5B1-62F0-4BFF-86AA-3627040FF4C2}"/>
+  <xr:revisionPtr revIDLastSave="97" documentId="8_{DCB34105-0091-4572-A59E-812606D8BD9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0C45C1EF-CBB7-410D-99CE-46EBC10F3BED}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{8C70E17E-B8BD-41DA-A72E-ED719EC33205}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{8C70E17E-B8BD-41DA-A72E-ED719EC33205}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="35">
   <si>
     <t>Estabelecimento</t>
   </si>
@@ -131,6 +131,18 @@
   </si>
   <si>
     <t>Metropoly</t>
+  </si>
+  <si>
+    <t>Don Hamburgo</t>
+  </si>
+  <si>
+    <t>L'Entrecôte de Paris</t>
+  </si>
+  <si>
+    <t>Bistrô Paris 6</t>
+  </si>
+  <si>
+    <t>Beco Hexagonal</t>
   </si>
 </sst>
 </file>
@@ -482,13 +494,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CDA3779-892F-4DE3-838B-C6C170BE1E7A}">
-  <dimension ref="A1:C25"/>
+  <dimension ref="A1:C29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="24.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.7109375" customWidth="1"/>
@@ -612,7 +624,7 @@
         <v>7</v>
       </c>
       <c r="C11" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -634,7 +646,7 @@
         <v>7</v>
       </c>
       <c r="C13" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -711,7 +723,7 @@
         <v>7</v>
       </c>
       <c r="C20" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -767,6 +779,50 @@
       </c>
       <c r="C25" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" t="s">
+        <v>31</v>
+      </c>
+      <c r="B26" t="s">
+        <v>7</v>
+      </c>
+      <c r="C26" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" t="s">
+        <v>32</v>
+      </c>
+      <c r="B27" t="s">
+        <v>7</v>
+      </c>
+      <c r="C27" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" t="s">
+        <v>33</v>
+      </c>
+      <c r="B28" t="s">
+        <v>7</v>
+      </c>
+      <c r="C28" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" t="s">
+        <v>34</v>
+      </c>
+      <c r="B29" t="s">
+        <v>4</v>
+      </c>
+      <c r="C29" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>